<commit_message>
feat: Suppport blog static field
</commit_message>
<xml_diff>
--- a/applications/DEMO/aspnet-core/src/DEMO.Domain.Shared/Files/CMS範例格式.xlsx
+++ b/applications/DEMO/aspnet-core/src/DEMO.Domain.Shared/Files/CMS範例格式.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static</t>
   </si>
   <si>
     <t xml:space="preserve">校園公告</t>
@@ -232,8 +235,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -330,13 +337,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.20703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="59.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.18"/>
@@ -352,61 +359,73 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
+      <c r="A4" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
+      <c r="A5" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
+      <c r="A6" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
+      <c r="A8" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -431,7 +450,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.20703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.98"/>
@@ -441,147 +460,147 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>38110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="n">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <v>43911</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="n">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <v>43912</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="n">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <v>43913</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="n">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <v>43914</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2" t="n">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="n">
         <v>43915</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2" t="n">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <v>43916</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2" t="n">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="n">
         <v>43917</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="2" t="n">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="n">
         <v>43918</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2" t="n">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <v>43920</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="n">
         <v>43921</v>
       </c>
     </row>

</xml_diff>